<commit_message>
Added the standard deviation functionality
</commit_message>
<xml_diff>
--- a/store_demand_df.xlsx
+++ b/store_demand_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L104"/>
+  <dimension ref="A1:M104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,40 +456,45 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>std_demand</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Warehouse</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>monthly_eoq</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>cycle_time</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>cycle_time_in_days</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>cycle_time_in_hr</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>full_cycles_in_lead_time</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>effective_lead_time</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>reorder_point</t>
         </is>
@@ -509,27 +514,30 @@
         <v>1710</v>
       </c>
       <c r="E2" t="n">
-        <v>106406</v>
+        <v>855</v>
       </c>
       <c r="F2" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G2" t="n">
         <v>184.9324200890693</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>0.108147614087175</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>3.24442842261525</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>77.86628214276601</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>18</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>0.05334294643084969</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>91.21643839675298</v>
       </c>
     </row>
@@ -547,27 +555,30 @@
         <v>2422.5</v>
       </c>
       <c r="E3" t="n">
-        <v>106406</v>
+        <v>855</v>
       </c>
       <c r="F3" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G3" t="n">
         <v>220.1136070305514</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>0.09086217008485092</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>2.725865102545528</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>65.42076246109266</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>22</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>0.001032258133279562</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>2.500645327869739</v>
       </c>
     </row>
@@ -585,27 +596,30 @@
         <v>1710</v>
       </c>
       <c r="E4" t="n">
-        <v>106406</v>
+        <v>1045</v>
       </c>
       <c r="F4" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G4" t="n">
         <v>184.9324200890693</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>0.108147614087175</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>3.24442842261525</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>77.86628214276601</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>18</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>0.05334294643084969</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>91.21643839675298</v>
       </c>
     </row>
@@ -623,27 +637,30 @@
         <v>1567.5</v>
       </c>
       <c r="E5" t="n">
-        <v>106406</v>
+        <v>1092.5</v>
       </c>
       <c r="F5" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G5" t="n">
         <v>177.0593120962577</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>0.112956498944981</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>3.388694968349431</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>81.32867924038634</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>17</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>0.07973951793532286</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>124.9916943636186</v>
       </c>
     </row>
@@ -661,27 +678,30 @@
         <v>3135</v>
       </c>
       <c r="E6" t="n">
-        <v>106406</v>
+        <v>1377.5</v>
       </c>
       <c r="F6" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G6" t="n">
         <v>250.3996805109783</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>0.07987230638308718</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>2.396169191492615</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>57.50806059582276</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>25</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>0.003192340422820461</v>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="n">
         <v>10.00798722554214</v>
       </c>
     </row>
@@ -699,27 +719,30 @@
         <v>2850</v>
       </c>
       <c r="E7" t="n">
-        <v>106406</v>
+        <v>1425</v>
       </c>
       <c r="F7" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G7" t="n">
         <v>238.7467277262664</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>0.08377078165833911</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>2.513123449750173</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>60.31496279400416</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>23</v>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>0.07327202185820059</v>
       </c>
-      <c r="L7" t="n">
+      <c r="M7" t="n">
         <v>208.8252622958717</v>
       </c>
     </row>
@@ -737,27 +760,30 @@
         <v>712.5</v>
       </c>
       <c r="E8" t="n">
-        <v>106406</v>
+        <v>1615</v>
       </c>
       <c r="F8" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G8" t="n">
         <v>119.3733638631332</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>0.1675415633166782</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>5.026246899500347</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>120.6299255880083</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>11</v>
       </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
         <v>0.1570428035165397</v>
       </c>
-      <c r="L8" t="n">
+      <c r="M8" t="n">
         <v>111.8929975055345</v>
       </c>
     </row>
@@ -775,27 +801,30 @@
         <v>2280</v>
       </c>
       <c r="E9" t="n">
-        <v>106406</v>
+        <v>1282.5</v>
       </c>
       <c r="F9" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G9" t="n">
         <v>213.5415650406262</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>0.09365858115816939</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>2.809757434745082</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>67.43417843388195</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>21</v>
       </c>
-      <c r="K9" t="n">
+      <c r="L9" t="n">
         <v>0.03316979567844291</v>
       </c>
-      <c r="L9" t="n">
+      <c r="M9" t="n">
         <v>75.62713414684984</v>
       </c>
     </row>
@@ -813,27 +842,30 @@
         <v>712.5</v>
       </c>
       <c r="E10" t="n">
-        <v>106406</v>
+        <v>1045</v>
       </c>
       <c r="F10" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G10" t="n">
         <v>119.3733638631332</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>0.1675415633166782</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>5.026246899500347</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>120.6299255880083</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>11</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>0.1570428035165397</v>
       </c>
-      <c r="L10" t="n">
+      <c r="M10" t="n">
         <v>111.8929975055345</v>
       </c>
     </row>
@@ -851,27 +883,30 @@
         <v>1710</v>
       </c>
       <c r="E11" t="n">
-        <v>106406</v>
+        <v>712.5</v>
       </c>
       <c r="F11" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G11" t="n">
         <v>184.9324200890693</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>0.108147614087175</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>3.24442842261525</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>77.86628214276601</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>18</v>
       </c>
-      <c r="K11" t="n">
+      <c r="L11" t="n">
         <v>0.05334294643084969</v>
       </c>
-      <c r="L11" t="n">
+      <c r="M11" t="n">
         <v>91.21643839675298</v>
       </c>
     </row>
@@ -889,27 +924,30 @@
         <v>997.5</v>
       </c>
       <c r="E12" t="n">
-        <v>106406</v>
+        <v>807.5</v>
       </c>
       <c r="F12" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G12" t="n">
         <v>141.2444689182553</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>0.1415984650809577</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>4.247953952428731</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>101.9508948582896</v>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
         <v>14</v>
       </c>
-      <c r="K12" t="n">
+      <c r="L12" t="n">
         <v>0.01762148886659198</v>
       </c>
-      <c r="L12" t="n">
+      <c r="M12" t="n">
         <v>17.5774351444255</v>
       </c>
     </row>
@@ -927,27 +965,30 @@
         <v>2565</v>
       </c>
       <c r="E13" t="n">
-        <v>106406</v>
+        <v>950</v>
       </c>
       <c r="F13" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G13" t="n">
         <v>226.4950330581225</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>0.08830215713766959</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>2.649064714130088</v>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>63.5775531391221</v>
       </c>
-      <c r="J13" t="n">
+      <c r="K13" t="n">
         <v>22</v>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>0.05735254297126913</v>
       </c>
-      <c r="L13" t="n">
+      <c r="M13" t="n">
         <v>147.1092727213053</v>
       </c>
     </row>
@@ -965,27 +1006,30 @@
         <v>2992.5</v>
       </c>
       <c r="E14" t="n">
-        <v>106406</v>
+        <v>997.5</v>
       </c>
       <c r="F14" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G14" t="n">
         <v>244.6425964545014</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>0.08175191193132877</v>
       </c>
-      <c r="H14" t="n">
+      <c r="I14" t="n">
         <v>2.452557357939863</v>
       </c>
-      <c r="I14" t="n">
+      <c r="J14" t="n">
         <v>58.86137659055672</v>
       </c>
-      <c r="J14" t="n">
+      <c r="K14" t="n">
         <v>24</v>
       </c>
-      <c r="K14" t="n">
+      <c r="L14" t="n">
         <v>0.03795411364810941</v>
       </c>
-      <c r="L14" t="n">
+      <c r="M14" t="n">
         <v>113.5776850919674</v>
       </c>
     </row>
@@ -1003,27 +1047,30 @@
         <v>1995</v>
       </c>
       <c r="E15" t="n">
-        <v>106406</v>
+        <v>1187.5</v>
       </c>
       <c r="F15" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G15" t="n">
         <v>199.7498435543818</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>0.1001252348643518</v>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
         <v>3.003757045930553</v>
       </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
         <v>72.09016910233328</v>
       </c>
-      <c r="J15" t="n">
+      <c r="K15" t="n">
         <v>19</v>
       </c>
-      <c r="K15" t="n">
+      <c r="L15" t="n">
         <v>0.09762053757731648</v>
       </c>
-      <c r="L15" t="n">
+      <c r="M15" t="n">
         <v>194.7529724667464</v>
       </c>
     </row>
@@ -1041,27 +1088,30 @@
         <v>855</v>
       </c>
       <c r="E16" t="n">
-        <v>106406</v>
+        <v>997.5</v>
       </c>
       <c r="F16" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G16" t="n">
         <v>130.7669683062202</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>0.1529438225803745</v>
       </c>
-      <c r="H16" t="n">
+      <c r="I16" t="n">
         <v>4.588314677411235</v>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>110.1195522578696</v>
       </c>
-      <c r="J16" t="n">
+      <c r="K16" t="n">
         <v>13</v>
       </c>
-      <c r="K16" t="n">
+      <c r="L16" t="n">
         <v>0.01173030645513151</v>
       </c>
-      <c r="L16" t="n">
+      <c r="M16" t="n">
         <v>10.02941201913744</v>
       </c>
     </row>
@@ -1079,27 +1129,30 @@
         <v>1995</v>
       </c>
       <c r="E17" t="n">
-        <v>106406</v>
+        <v>997.5</v>
       </c>
       <c r="F17" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G17" t="n">
         <v>199.7498435543818</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>0.1001252348643518</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>3.003757045930553</v>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>72.09016910233328</v>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
         <v>19</v>
       </c>
-      <c r="K17" t="n">
+      <c r="L17" t="n">
         <v>0.09762053757731648</v>
       </c>
-      <c r="L17" t="n">
+      <c r="M17" t="n">
         <v>194.7529724667464</v>
       </c>
     </row>
@@ -1117,27 +1170,30 @@
         <v>1852.5</v>
       </c>
       <c r="E18" t="n">
-        <v>106406</v>
+        <v>807.5</v>
       </c>
       <c r="F18" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G18" t="n">
         <v>192.4837655492016</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>0.1039048666932262</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>3.117146000796786</v>
       </c>
-      <c r="I18" t="n">
+      <c r="J18" t="n">
         <v>74.81150401912286</v>
       </c>
-      <c r="J18" t="n">
+      <c r="K18" t="n">
         <v>19</v>
       </c>
-      <c r="K18" t="n">
+      <c r="L18" t="n">
         <v>0.02580753282870196</v>
       </c>
-      <c r="L18" t="n">
+      <c r="M18" t="n">
         <v>47.80845456517039</v>
       </c>
     </row>
@@ -1155,27 +1211,30 @@
         <v>1852.5</v>
       </c>
       <c r="E19" t="n">
-        <v>106406</v>
+        <v>807.5</v>
       </c>
       <c r="F19" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G19" t="n">
         <v>192.4837655492016</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>0.1039048666932262</v>
       </c>
-      <c r="H19" t="n">
+      <c r="I19" t="n">
         <v>3.117146000796786</v>
       </c>
-      <c r="I19" t="n">
+      <c r="J19" t="n">
         <v>74.81150401912286</v>
       </c>
-      <c r="J19" t="n">
+      <c r="K19" t="n">
         <v>19</v>
       </c>
-      <c r="K19" t="n">
+      <c r="L19" t="n">
         <v>0.02580753282870196</v>
       </c>
-      <c r="L19" t="n">
+      <c r="M19" t="n">
         <v>47.80845456517039</v>
       </c>
     </row>
@@ -1193,27 +1252,30 @@
         <v>1140</v>
       </c>
       <c r="E20" t="n">
-        <v>106406</v>
+        <v>902.5</v>
       </c>
       <c r="F20" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G20" t="n">
         <v>150.996688705415</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>0.1324532357065044</v>
       </c>
-      <c r="H20" t="n">
+      <c r="I20" t="n">
         <v>3.973597071195131</v>
       </c>
-      <c r="I20" t="n">
+      <c r="J20" t="n">
         <v>95.36632970868314</v>
       </c>
-      <c r="J20" t="n">
+      <c r="K20" t="n">
         <v>15</v>
       </c>
-      <c r="K20" t="n">
+      <c r="L20" t="n">
         <v>0.01320146440243475</v>
       </c>
-      <c r="L20" t="n">
+      <c r="M20" t="n">
         <v>15.04966941877561</v>
       </c>
     </row>
@@ -1231,27 +1293,30 @@
         <v>1425</v>
       </c>
       <c r="E21" t="n">
-        <v>106406</v>
+        <v>997.5</v>
       </c>
       <c r="F21" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G21" t="n">
         <v>168.8194301613413</v>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>0.1184697755518185</v>
       </c>
-      <c r="H21" t="n">
+      <c r="I21" t="n">
         <v>3.554093266554554</v>
       </c>
-      <c r="I21" t="n">
+      <c r="J21" t="n">
         <v>85.29823839730931</v>
       </c>
-      <c r="J21" t="n">
+      <c r="K21" t="n">
         <v>16</v>
       </c>
-      <c r="K21" t="n">
+      <c r="L21" t="n">
         <v>0.1044835911709043</v>
       </c>
-      <c r="L21" t="n">
+      <c r="M21" t="n">
         <v>148.8891174185387</v>
       </c>
     </row>
@@ -1269,27 +1334,30 @@
         <v>2707.5</v>
       </c>
       <c r="E22" t="n">
-        <v>106406</v>
+        <v>1187.5</v>
       </c>
       <c r="F22" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G22" t="n">
         <v>232.7015255644019</v>
       </c>
-      <c r="G22" t="n">
+      <c r="H22" t="n">
         <v>0.085947008518708</v>
       </c>
-      <c r="H22" t="n">
+      <c r="I22" t="n">
         <v>2.57841025556124</v>
       </c>
-      <c r="I22" t="n">
+      <c r="J22" t="n">
         <v>61.88184613346976</v>
       </c>
-      <c r="J22" t="n">
+      <c r="K22" t="n">
         <v>23</v>
       </c>
-      <c r="K22" t="n">
+      <c r="L22" t="n">
         <v>0.0232188040697161</v>
       </c>
-      <c r="L22" t="n">
+      <c r="M22" t="n">
         <v>62.86491201875635</v>
       </c>
     </row>
@@ -1307,27 +1375,30 @@
         <v>712.5</v>
       </c>
       <c r="E23" t="n">
-        <v>106406</v>
+        <v>1520</v>
       </c>
       <c r="F23" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G23" t="n">
         <v>119.3733638631332</v>
       </c>
-      <c r="G23" t="n">
+      <c r="H23" t="n">
         <v>0.1675415633166782</v>
       </c>
-      <c r="H23" t="n">
+      <c r="I23" t="n">
         <v>5.026246899500347</v>
       </c>
-      <c r="I23" t="n">
+      <c r="J23" t="n">
         <v>120.6299255880083</v>
       </c>
-      <c r="J23" t="n">
+      <c r="K23" t="n">
         <v>11</v>
       </c>
-      <c r="K23" t="n">
+      <c r="L23" t="n">
         <v>0.1570428035165397</v>
       </c>
-      <c r="L23" t="n">
+      <c r="M23" t="n">
         <v>111.8929975055345</v>
       </c>
     </row>
@@ -1345,27 +1416,30 @@
         <v>1710</v>
       </c>
       <c r="E24" t="n">
-        <v>106406</v>
+        <v>1425</v>
       </c>
       <c r="F24" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G24" t="n">
         <v>184.9324200890693</v>
       </c>
-      <c r="G24" t="n">
+      <c r="H24" t="n">
         <v>0.108147614087175</v>
       </c>
-      <c r="H24" t="n">
+      <c r="I24" t="n">
         <v>3.24442842261525</v>
       </c>
-      <c r="I24" t="n">
+      <c r="J24" t="n">
         <v>77.86628214276601</v>
       </c>
-      <c r="J24" t="n">
+      <c r="K24" t="n">
         <v>18</v>
       </c>
-      <c r="K24" t="n">
+      <c r="L24" t="n">
         <v>0.05334294643084969</v>
       </c>
-      <c r="L24" t="n">
+      <c r="M24" t="n">
         <v>91.21643839675298</v>
       </c>
     </row>
@@ -1383,27 +1457,30 @@
         <v>1995</v>
       </c>
       <c r="E25" t="n">
-        <v>106406</v>
+        <v>1425</v>
       </c>
       <c r="F25" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G25" t="n">
         <v>199.7498435543818</v>
       </c>
-      <c r="G25" t="n">
+      <c r="H25" t="n">
         <v>0.1001252348643518</v>
       </c>
-      <c r="H25" t="n">
+      <c r="I25" t="n">
         <v>3.003757045930553</v>
       </c>
-      <c r="I25" t="n">
+      <c r="J25" t="n">
         <v>72.09016910233328</v>
       </c>
-      <c r="J25" t="n">
+      <c r="K25" t="n">
         <v>19</v>
       </c>
-      <c r="K25" t="n">
+      <c r="L25" t="n">
         <v>0.09762053757731648</v>
       </c>
-      <c r="L25" t="n">
+      <c r="M25" t="n">
         <v>194.7529724667464</v>
       </c>
     </row>
@@ -1421,27 +1498,30 @@
         <v>3135</v>
       </c>
       <c r="E26" t="n">
-        <v>106406</v>
+        <v>997.5</v>
       </c>
       <c r="F26" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G26" t="n">
         <v>250.3996805109783</v>
       </c>
-      <c r="G26" t="n">
+      <c r="H26" t="n">
         <v>0.07987230638308718</v>
       </c>
-      <c r="H26" t="n">
+      <c r="I26" t="n">
         <v>2.396169191492615</v>
       </c>
-      <c r="I26" t="n">
+      <c r="J26" t="n">
         <v>57.50806059582276</v>
       </c>
-      <c r="J26" t="n">
+      <c r="K26" t="n">
         <v>25</v>
       </c>
-      <c r="K26" t="n">
+      <c r="L26" t="n">
         <v>0.003192340422820461</v>
       </c>
-      <c r="L26" t="n">
+      <c r="M26" t="n">
         <v>10.00798722554214</v>
       </c>
     </row>
@@ -1459,27 +1539,30 @@
         <v>712.5</v>
       </c>
       <c r="E27" t="n">
-        <v>106406</v>
+        <v>950</v>
       </c>
       <c r="F27" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G27" t="n">
         <v>119.3733638631332</v>
       </c>
-      <c r="G27" t="n">
+      <c r="H27" t="n">
         <v>0.1675415633166782</v>
       </c>
-      <c r="H27" t="n">
+      <c r="I27" t="n">
         <v>5.026246899500347</v>
       </c>
-      <c r="I27" t="n">
+      <c r="J27" t="n">
         <v>120.6299255880083</v>
       </c>
-      <c r="J27" t="n">
+      <c r="K27" t="n">
         <v>11</v>
       </c>
-      <c r="K27" t="n">
+      <c r="L27" t="n">
         <v>0.1570428035165397</v>
       </c>
-      <c r="L27" t="n">
+      <c r="M27" t="n">
         <v>111.8929975055345</v>
       </c>
     </row>
@@ -1497,27 +1580,30 @@
         <v>1282.5</v>
       </c>
       <c r="E28" t="n">
-        <v>106406</v>
+        <v>855</v>
       </c>
       <c r="F28" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G28" t="n">
         <v>160.1561737804697</v>
       </c>
-      <c r="G28" t="n">
+      <c r="H28" t="n">
         <v>0.1248781082108925</v>
       </c>
-      <c r="H28" t="n">
+      <c r="I28" t="n">
         <v>3.746343246326776</v>
       </c>
-      <c r="I28" t="n">
+      <c r="J28" t="n">
         <v>89.91223791184262</v>
       </c>
-      <c r="J28" t="n">
+      <c r="K28" t="n">
         <v>16</v>
       </c>
-      <c r="K28" t="n">
+      <c r="L28" t="n">
         <v>0.001950268625719564</v>
       </c>
-      <c r="L28" t="n">
+      <c r="M28" t="n">
         <v>2.501219512485342</v>
       </c>
     </row>
@@ -1535,27 +1621,30 @@
         <v>997.5</v>
       </c>
       <c r="E29" t="n">
-        <v>106406</v>
+        <v>950</v>
       </c>
       <c r="F29" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G29" t="n">
         <v>141.2444689182553</v>
       </c>
-      <c r="G29" t="n">
+      <c r="H29" t="n">
         <v>0.1415984650809577</v>
       </c>
-      <c r="H29" t="n">
+      <c r="I29" t="n">
         <v>4.247953952428731</v>
       </c>
-      <c r="I29" t="n">
+      <c r="J29" t="n">
         <v>101.9508948582896</v>
       </c>
-      <c r="J29" t="n">
+      <c r="K29" t="n">
         <v>14</v>
       </c>
-      <c r="K29" t="n">
+      <c r="L29" t="n">
         <v>0.01762148886659198</v>
       </c>
-      <c r="L29" t="n">
+      <c r="M29" t="n">
         <v>17.5774351444255</v>
       </c>
     </row>
@@ -1573,27 +1662,30 @@
         <v>2422.5</v>
       </c>
       <c r="E30" t="n">
-        <v>106406</v>
+        <v>1092.5</v>
       </c>
       <c r="F30" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G30" t="n">
         <v>220.1136070305514</v>
       </c>
-      <c r="G30" t="n">
+      <c r="H30" t="n">
         <v>0.09086217008485092</v>
       </c>
-      <c r="H30" t="n">
+      <c r="I30" t="n">
         <v>2.725865102545528</v>
       </c>
-      <c r="I30" t="n">
+      <c r="J30" t="n">
         <v>65.42076246109266</v>
       </c>
-      <c r="J30" t="n">
+      <c r="K30" t="n">
         <v>22</v>
       </c>
-      <c r="K30" t="n">
+      <c r="L30" t="n">
         <v>0.001032258133279562</v>
       </c>
-      <c r="L30" t="n">
+      <c r="M30" t="n">
         <v>2.500645327869739</v>
       </c>
     </row>
@@ -1611,27 +1703,30 @@
         <v>997.5</v>
       </c>
       <c r="E31" t="n">
-        <v>106406</v>
+        <v>950</v>
       </c>
       <c r="F31" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G31" t="n">
         <v>141.2444689182553</v>
       </c>
-      <c r="G31" t="n">
+      <c r="H31" t="n">
         <v>0.1415984650809577</v>
       </c>
-      <c r="H31" t="n">
+      <c r="I31" t="n">
         <v>4.247953952428731</v>
       </c>
-      <c r="I31" t="n">
+      <c r="J31" t="n">
         <v>101.9508948582896</v>
       </c>
-      <c r="J31" t="n">
+      <c r="K31" t="n">
         <v>14</v>
       </c>
-      <c r="K31" t="n">
+      <c r="L31" t="n">
         <v>0.01762148886659198</v>
       </c>
-      <c r="L31" t="n">
+      <c r="M31" t="n">
         <v>17.5774351444255</v>
       </c>
     </row>
@@ -1649,27 +1744,30 @@
         <v>1567.5</v>
       </c>
       <c r="E32" t="n">
-        <v>106406</v>
+        <v>902.5</v>
       </c>
       <c r="F32" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G32" t="n">
         <v>177.0593120962577</v>
       </c>
-      <c r="G32" t="n">
+      <c r="H32" t="n">
         <v>0.112956498944981</v>
       </c>
-      <c r="H32" t="n">
+      <c r="I32" t="n">
         <v>3.388694968349431</v>
       </c>
-      <c r="I32" t="n">
+      <c r="J32" t="n">
         <v>81.32867924038634</v>
       </c>
-      <c r="J32" t="n">
+      <c r="K32" t="n">
         <v>17</v>
       </c>
-      <c r="K32" t="n">
+      <c r="L32" t="n">
         <v>0.07973951793532286</v>
       </c>
-      <c r="L32" t="n">
+      <c r="M32" t="n">
         <v>124.9916943636186</v>
       </c>
     </row>
@@ -1687,27 +1785,30 @@
         <v>1282.5</v>
       </c>
       <c r="E33" t="n">
-        <v>106406</v>
+        <v>807.5</v>
       </c>
       <c r="F33" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G33" t="n">
         <v>160.1561737804697</v>
       </c>
-      <c r="G33" t="n">
+      <c r="H33" t="n">
         <v>0.1248781082108925</v>
       </c>
-      <c r="H33" t="n">
+      <c r="I33" t="n">
         <v>3.746343246326776</v>
       </c>
-      <c r="I33" t="n">
+      <c r="J33" t="n">
         <v>89.91223791184262</v>
       </c>
-      <c r="J33" t="n">
+      <c r="K33" t="n">
         <v>16</v>
       </c>
-      <c r="K33" t="n">
+      <c r="L33" t="n">
         <v>0.001950268625719564</v>
       </c>
-      <c r="L33" t="n">
+      <c r="M33" t="n">
         <v>2.501219512485342</v>
       </c>
     </row>
@@ -1725,27 +1826,30 @@
         <v>1567.5</v>
       </c>
       <c r="E34" t="n">
-        <v>106406</v>
+        <v>997.5</v>
       </c>
       <c r="F34" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G34" t="n">
         <v>177.0593120962577</v>
       </c>
-      <c r="G34" t="n">
+      <c r="H34" t="n">
         <v>0.112956498944981</v>
       </c>
-      <c r="H34" t="n">
+      <c r="I34" t="n">
         <v>3.388694968349431</v>
       </c>
-      <c r="I34" t="n">
+      <c r="J34" t="n">
         <v>81.32867924038634</v>
       </c>
-      <c r="J34" t="n">
+      <c r="K34" t="n">
         <v>17</v>
       </c>
-      <c r="K34" t="n">
+      <c r="L34" t="n">
         <v>0.07973951793532286</v>
       </c>
-      <c r="L34" t="n">
+      <c r="M34" t="n">
         <v>124.9916943636186</v>
       </c>
     </row>
@@ -1763,27 +1867,30 @@
         <v>997.5</v>
       </c>
       <c r="E35" t="n">
-        <v>106406</v>
+        <v>1187.5</v>
       </c>
       <c r="F35" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G35" t="n">
         <v>141.2444689182553</v>
       </c>
-      <c r="G35" t="n">
+      <c r="H35" t="n">
         <v>0.1415984650809577</v>
       </c>
-      <c r="H35" t="n">
+      <c r="I35" t="n">
         <v>4.247953952428731</v>
       </c>
-      <c r="I35" t="n">
+      <c r="J35" t="n">
         <v>101.9508948582896</v>
       </c>
-      <c r="J35" t="n">
+      <c r="K35" t="n">
         <v>14</v>
       </c>
-      <c r="K35" t="n">
+      <c r="L35" t="n">
         <v>0.01762148886659198</v>
       </c>
-      <c r="L35" t="n">
+      <c r="M35" t="n">
         <v>17.5774351444255</v>
       </c>
     </row>
@@ -1801,27 +1908,30 @@
         <v>13110</v>
       </c>
       <c r="E36" t="n">
-        <v>106406</v>
+        <v>1187.5</v>
       </c>
       <c r="F36" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G36" t="n">
         <v>512.0546845796844</v>
       </c>
-      <c r="G36" t="n">
+      <c r="H36" t="n">
         <v>0.03905832834322535</v>
       </c>
-      <c r="H36" t="n">
+      <c r="I36" t="n">
         <v>1.171749850296761</v>
       </c>
-      <c r="I36" t="n">
+      <c r="J36" t="n">
         <v>28.12199640712226</v>
       </c>
-      <c r="J36" t="n">
+      <c r="K36" t="n">
         <v>76</v>
       </c>
-      <c r="K36" t="n">
+      <c r="L36" t="n">
         <v>0.03156704591487314</v>
       </c>
-      <c r="L36" t="n">
+      <c r="M36" t="n">
         <v>413.8439719439868</v>
       </c>
     </row>
@@ -1839,27 +1949,30 @@
         <v>4845</v>
       </c>
       <c r="E37" t="n">
-        <v>106406</v>
+        <v>1377.5</v>
       </c>
       <c r="F37" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G37" t="n">
         <v>311.2876483254676</v>
       </c>
-      <c r="G37" t="n">
+      <c r="H37" t="n">
         <v>0.06424925662032355</v>
       </c>
-      <c r="H37" t="n">
+      <c r="I37" t="n">
         <v>1.927477698609706</v>
       </c>
-      <c r="I37" t="n">
+      <c r="J37" t="n">
         <v>46.25946476663295</v>
       </c>
-      <c r="J37" t="n">
+      <c r="K37" t="n">
         <v>46</v>
       </c>
-      <c r="K37" t="n">
+      <c r="L37" t="n">
         <v>0.04453419546511661</v>
       </c>
-      <c r="L37" t="n">
+      <c r="M37" t="n">
         <v>215.76817702849</v>
       </c>
     </row>
@@ -1877,27 +1990,30 @@
         <v>855</v>
       </c>
       <c r="E38" t="n">
-        <v>106406</v>
+        <v>1140</v>
       </c>
       <c r="F38" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G38" t="n">
         <v>130.7669683062202</v>
       </c>
-      <c r="G38" t="n">
+      <c r="H38" t="n">
         <v>0.1529438225803745</v>
       </c>
-      <c r="H38" t="n">
+      <c r="I38" t="n">
         <v>4.588314677411235</v>
       </c>
-      <c r="I38" t="n">
+      <c r="J38" t="n">
         <v>110.1195522578696</v>
       </c>
-      <c r="J38" t="n">
+      <c r="K38" t="n">
         <v>19</v>
       </c>
-      <c r="K38" t="n">
+      <c r="L38" t="n">
         <v>0.09406737097288431</v>
       </c>
-      <c r="L38" t="n">
+      <c r="M38" t="n">
         <v>80.42760218181608</v>
       </c>
     </row>
@@ -1915,27 +2031,30 @@
         <v>2351.25</v>
       </c>
       <c r="E39" t="n">
-        <v>106406</v>
+        <v>1377.5</v>
       </c>
       <c r="F39" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G39" t="n">
         <v>216.8524844220144</v>
       </c>
-      <c r="G39" t="n">
+      <c r="H39" t="n">
         <v>0.0922285951821433</v>
       </c>
-      <c r="H39" t="n">
+      <c r="I39" t="n">
         <v>2.766857855464299</v>
       </c>
-      <c r="I39" t="n">
+      <c r="J39" t="n">
         <v>66.40458853114318</v>
       </c>
-      <c r="J39" t="n">
+      <c r="K39" t="n">
         <v>32</v>
       </c>
-      <c r="K39" t="n">
+      <c r="L39" t="n">
         <v>0.0486849541714145</v>
       </c>
-      <c r="L39" t="n">
+      <c r="M39" t="n">
         <v>114.4704984955383</v>
       </c>
     </row>
@@ -1953,27 +2072,30 @@
         <v>1567.5</v>
       </c>
       <c r="E40" t="n">
-        <v>106406</v>
+        <v>1472.5</v>
       </c>
       <c r="F40" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G40" t="n">
         <v>177.0593120962577</v>
       </c>
-      <c r="G40" t="n">
+      <c r="H40" t="n">
         <v>0.112956498944981</v>
       </c>
-      <c r="H40" t="n">
+      <c r="I40" t="n">
         <v>3.388694968349431</v>
       </c>
-      <c r="I40" t="n">
+      <c r="J40" t="n">
         <v>81.32867924038634</v>
       </c>
-      <c r="J40" t="n">
+      <c r="K40" t="n">
         <v>26</v>
       </c>
-      <c r="K40" t="n">
+      <c r="L40" t="n">
         <v>0.0631310274304937</v>
       </c>
-      <c r="L40" t="n">
+      <c r="M40" t="n">
         <v>98.95788549729888</v>
       </c>
     </row>
@@ -1991,27 +2113,30 @@
         <v>2137.5</v>
       </c>
       <c r="E41" t="n">
-        <v>106406</v>
+        <v>1615</v>
       </c>
       <c r="F41" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G41" t="n">
         <v>206.7607312813533</v>
       </c>
-      <c r="G41" t="n">
+      <c r="H41" t="n">
         <v>0.09673016668133488</v>
       </c>
-      <c r="H41" t="n">
+      <c r="I41" t="n">
         <v>2.901905000440046</v>
       </c>
-      <c r="I41" t="n">
+      <c r="J41" t="n">
         <v>69.64572001056112</v>
       </c>
-      <c r="J41" t="n">
+      <c r="K41" t="n">
         <v>31</v>
       </c>
-      <c r="K41" t="n">
+      <c r="L41" t="n">
         <v>0.00136483287861866</v>
       </c>
-      <c r="L41" t="n">
+      <c r="M41" t="n">
         <v>2.917330278047387</v>
       </c>
     </row>
@@ -2029,27 +2154,30 @@
         <v>2137.5</v>
       </c>
       <c r="E42" t="n">
-        <v>106406</v>
+        <v>1710</v>
       </c>
       <c r="F42" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G42" t="n">
         <v>206.7607312813533</v>
       </c>
-      <c r="G42" t="n">
+      <c r="H42" t="n">
         <v>0.09673016668133488</v>
       </c>
-      <c r="H42" t="n">
+      <c r="I42" t="n">
         <v>2.901905000440046</v>
       </c>
-      <c r="I42" t="n">
+      <c r="J42" t="n">
         <v>69.64572001056112</v>
       </c>
-      <c r="J42" t="n">
+      <c r="K42" t="n">
         <v>31</v>
       </c>
-      <c r="K42" t="n">
+      <c r="L42" t="n">
         <v>0.00136483287861866</v>
       </c>
-      <c r="L42" t="n">
+      <c r="M42" t="n">
         <v>2.917330278047387</v>
       </c>
     </row>
@@ -2067,27 +2195,30 @@
         <v>4702.5</v>
       </c>
       <c r="E43" t="n">
-        <v>106406</v>
+        <v>1282.5</v>
       </c>
       <c r="F43" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G43" t="n">
         <v>306.6757245039131</v>
       </c>
-      <c r="G43" t="n">
+      <c r="H43" t="n">
         <v>0.06521546507260247</v>
       </c>
-      <c r="H43" t="n">
+      <c r="I43" t="n">
         <v>1.956463952178074</v>
       </c>
-      <c r="I43" t="n">
+      <c r="J43" t="n">
         <v>46.95513485227377</v>
       </c>
-      <c r="J43" t="n">
+      <c r="K43" t="n">
         <v>46</v>
       </c>
-      <c r="K43" t="n">
+      <c r="L43" t="n">
         <v>8.860666028676079e-05</v>
       </c>
-      <c r="L43" t="n">
+      <c r="M43" t="n">
         <v>0.4166728199984926</v>
       </c>
     </row>
@@ -2105,27 +2236,30 @@
         <v>8122.5</v>
       </c>
       <c r="E44" t="n">
-        <v>106406</v>
+        <v>1330</v>
       </c>
       <c r="F44" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G44" t="n">
         <v>403.0508652763321</v>
       </c>
-      <c r="G44" t="n">
+      <c r="H44" t="n">
         <v>0.04962152850431913</v>
       </c>
-      <c r="H44" t="n">
+      <c r="I44" t="n">
         <v>1.488645855129574</v>
       </c>
-      <c r="I44" t="n">
+      <c r="J44" t="n">
         <v>35.72750052310977</v>
       </c>
-      <c r="J44" t="n">
+      <c r="K44" t="n">
         <v>60</v>
       </c>
-      <c r="K44" t="n">
+      <c r="L44" t="n">
         <v>0.02270828974085237</v>
       </c>
-      <c r="L44" t="n">
+      <c r="M44" t="n">
         <v>184.4480834200734</v>
       </c>
     </row>
@@ -2143,27 +2277,30 @@
         <v>3705</v>
       </c>
       <c r="E45" t="n">
-        <v>106406</v>
+        <v>997.5</v>
       </c>
       <c r="F45" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G45" t="n">
         <v>272.213151776324</v>
       </c>
-      <c r="G45" t="n">
+      <c r="H45" t="n">
         <v>0.0734718358370645</v>
       </c>
-      <c r="H45" t="n">
+      <c r="I45" t="n">
         <v>2.204155075111935</v>
       </c>
-      <c r="I45" t="n">
+      <c r="J45" t="n">
         <v>52.89972180268644</v>
       </c>
-      <c r="J45" t="n">
+      <c r="K45" t="n">
         <v>40</v>
       </c>
-      <c r="K45" t="n">
+      <c r="L45" t="n">
         <v>0.06112656651741988</v>
       </c>
-      <c r="L45" t="n">
+      <c r="M45" t="n">
         <v>226.4739289470407</v>
       </c>
     </row>
@@ -2181,27 +2318,30 @@
         <v>2992.5</v>
       </c>
       <c r="E46" t="n">
-        <v>106406</v>
+        <v>1140</v>
       </c>
       <c r="F46" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G46" t="n">
         <v>244.6425964545014</v>
       </c>
-      <c r="G46" t="n">
+      <c r="H46" t="n">
         <v>0.08175191193132877</v>
       </c>
-      <c r="H46" t="n">
+      <c r="I46" t="n">
         <v>2.452557357939863</v>
       </c>
-      <c r="I46" t="n">
+      <c r="J46" t="n">
         <v>58.86137659055672</v>
       </c>
-      <c r="J46" t="n">
+      <c r="K46" t="n">
         <v>36</v>
       </c>
-      <c r="K46" t="n">
+      <c r="L46" t="n">
         <v>0.05693117047216401</v>
       </c>
-      <c r="L46" t="n">
+      <c r="M46" t="n">
         <v>170.3665276379508</v>
       </c>
     </row>
@@ -2219,27 +2359,30 @@
         <v>2850</v>
       </c>
       <c r="E47" t="n">
-        <v>106406</v>
+        <v>1140</v>
       </c>
       <c r="F47" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G47" t="n">
         <v>238.7467277262664</v>
       </c>
-      <c r="G47" t="n">
+      <c r="H47" t="n">
         <v>0.08377078165833911</v>
       </c>
-      <c r="H47" t="n">
+      <c r="I47" t="n">
         <v>2.513123449750173</v>
       </c>
-      <c r="I47" t="n">
+      <c r="J47" t="n">
         <v>60.31496279400416</v>
       </c>
-      <c r="J47" t="n">
+      <c r="K47" t="n">
         <v>35</v>
       </c>
-      <c r="K47" t="n">
+      <c r="L47" t="n">
         <v>0.06802264195813112</v>
       </c>
-      <c r="L47" t="n">
+      <c r="M47" t="n">
         <v>193.8645295806737</v>
       </c>
     </row>
@@ -2257,27 +2400,30 @@
         <v>7125</v>
       </c>
       <c r="E48" t="n">
-        <v>106406</v>
+        <v>1140</v>
       </c>
       <c r="F48" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G48" t="n">
         <v>377.4917217635375</v>
       </c>
-      <c r="G48" t="n">
+      <c r="H48" t="n">
         <v>0.05298129428260175</v>
       </c>
-      <c r="H48" t="n">
+      <c r="I48" t="n">
         <v>1.589438828478053</v>
       </c>
-      <c r="I48" t="n">
+      <c r="J48" t="n">
         <v>38.14653188347326</v>
       </c>
-      <c r="J48" t="n">
+      <c r="K48" t="n">
         <v>56</v>
       </c>
-      <c r="K48" t="n">
+      <c r="L48" t="n">
         <v>0.03304752017430168</v>
       </c>
-      <c r="L48" t="n">
+      <c r="M48" t="n">
         <v>235.4635812418995</v>
       </c>
     </row>
@@ -2295,27 +2441,30 @@
         <v>4275</v>
       </c>
       <c r="E49" t="n">
-        <v>106406</v>
+        <v>1282.5</v>
       </c>
       <c r="F49" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G49" t="n">
         <v>292.4038303442689</v>
       </c>
-      <c r="G49" t="n">
+      <c r="H49" t="n">
         <v>0.06839855680567694</v>
       </c>
-      <c r="H49" t="n">
+      <c r="I49" t="n">
         <v>2.051956704170308</v>
       </c>
-      <c r="I49" t="n">
+      <c r="J49" t="n">
         <v>49.2469609000874</v>
       </c>
-      <c r="J49" t="n">
+      <c r="K49" t="n">
         <v>43</v>
       </c>
-      <c r="K49" t="n">
+      <c r="L49" t="n">
         <v>0.05886205735589156</v>
       </c>
-      <c r="L49" t="n">
+      <c r="M49" t="n">
         <v>251.6352951964364</v>
       </c>
     </row>
@@ -2333,27 +2482,30 @@
         <v>2280</v>
       </c>
       <c r="E50" t="n">
-        <v>106406</v>
+        <v>1282.5</v>
       </c>
       <c r="F50" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G50" t="n">
         <v>213.5415650406262</v>
       </c>
-      <c r="G50" t="n">
+      <c r="H50" t="n">
         <v>0.09365858115816939</v>
       </c>
-      <c r="H50" t="n">
+      <c r="I50" t="n">
         <v>2.809757434745082</v>
       </c>
-      <c r="I50" t="n">
+      <c r="J50" t="n">
         <v>67.43417843388195</v>
       </c>
-      <c r="J50" t="n">
+      <c r="K50" t="n">
         <v>32</v>
       </c>
-      <c r="K50" t="n">
+      <c r="L50" t="n">
         <v>0.00292540293857968</v>
       </c>
-      <c r="L50" t="n">
+      <c r="M50" t="n">
         <v>6.66991869996167</v>
       </c>
     </row>
@@ -2371,27 +2523,30 @@
         <v>13252.5</v>
       </c>
       <c r="E51" t="n">
-        <v>106406</v>
+        <v>1472.5</v>
       </c>
       <c r="F51" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G51" t="n">
         <v>514.8300690519154</v>
       </c>
-      <c r="G51" t="n">
+      <c r="H51" t="n">
         <v>0.03884776978320433</v>
       </c>
-      <c r="H51" t="n">
+      <c r="I51" t="n">
         <v>1.16543309349613</v>
       </c>
-      <c r="I51" t="n">
+      <c r="J51" t="n">
         <v>27.97039424390712</v>
       </c>
-      <c r="J51" t="n">
+      <c r="K51" t="n">
         <v>77</v>
       </c>
-      <c r="K51" t="n">
+      <c r="L51" t="n">
         <v>0.008721726693266429</v>
       </c>
-      <c r="L51" t="n">
+      <c r="M51" t="n">
         <v>115.5846830025134</v>
       </c>
     </row>
@@ -2409,27 +2564,30 @@
         <v>2137.5</v>
       </c>
       <c r="E52" t="n">
-        <v>106406</v>
+        <v>1282.5</v>
       </c>
       <c r="F52" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G52" t="n">
         <v>206.7607312813533</v>
       </c>
-      <c r="G52" t="n">
+      <c r="H52" t="n">
         <v>0.09673016668133488</v>
       </c>
-      <c r="H52" t="n">
+      <c r="I52" t="n">
         <v>2.901905000440046</v>
       </c>
-      <c r="I52" t="n">
+      <c r="J52" t="n">
         <v>69.64572001056112</v>
       </c>
-      <c r="J52" t="n">
+      <c r="K52" t="n">
         <v>31</v>
       </c>
-      <c r="K52" t="n">
+      <c r="L52" t="n">
         <v>0.00136483287861866</v>
       </c>
-      <c r="L52" t="n">
+      <c r="M52" t="n">
         <v>2.917330278047387</v>
       </c>
     </row>
@@ -2447,27 +2605,30 @@
         <v>3277.5</v>
       </c>
       <c r="E53" t="n">
-        <v>106406</v>
+        <v>6127.5</v>
       </c>
       <c r="F53" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G53" t="n">
         <v>256.0273422898422</v>
       </c>
-      <c r="G53" t="n">
+      <c r="H53" t="n">
         <v>0.07811665668645071</v>
       </c>
-      <c r="H53" t="n">
+      <c r="I53" t="n">
         <v>2.343499700593521</v>
       </c>
-      <c r="I53" t="n">
+      <c r="J53" t="n">
         <v>56.24399281424451</v>
       </c>
-      <c r="J53" t="n">
+      <c r="K53" t="n">
         <v>38</v>
       </c>
-      <c r="K53" t="n">
+      <c r="L53" t="n">
         <v>0.03156704591487314</v>
       </c>
-      <c r="L53" t="n">
+      <c r="M53" t="n">
         <v>103.4609929859967</v>
       </c>
     </row>
@@ -2485,27 +2646,30 @@
         <v>2280</v>
       </c>
       <c r="E54" t="n">
-        <v>106406</v>
+        <v>6555</v>
       </c>
       <c r="F54" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G54" t="n">
         <v>213.5415650406262</v>
       </c>
-      <c r="G54" t="n">
+      <c r="H54" t="n">
         <v>0.09365858115816939</v>
       </c>
-      <c r="H54" t="n">
+      <c r="I54" t="n">
         <v>2.809757434745082</v>
       </c>
-      <c r="I54" t="n">
+      <c r="J54" t="n">
         <v>67.43417843388195</v>
       </c>
-      <c r="J54" t="n">
+      <c r="K54" t="n">
         <v>32</v>
       </c>
-      <c r="K54" t="n">
+      <c r="L54" t="n">
         <v>0.00292540293857968</v>
       </c>
-      <c r="L54" t="n">
+      <c r="M54" t="n">
         <v>6.66991869996167</v>
       </c>
     </row>
@@ -2523,27 +2687,30 @@
         <v>9405</v>
       </c>
       <c r="E55" t="n">
-        <v>106406</v>
+        <v>5985</v>
       </c>
       <c r="F55" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G55" t="n">
         <v>433.7049688440288</v>
       </c>
-      <c r="G55" t="n">
+      <c r="H55" t="n">
         <v>0.04611429759107165</v>
       </c>
-      <c r="H55" t="n">
+      <c r="I55" t="n">
         <v>1.383428927732149</v>
       </c>
-      <c r="I55" t="n">
+      <c r="J55" t="n">
         <v>33.20229426557159</v>
       </c>
-      <c r="J55" t="n">
+      <c r="K55" t="n">
         <v>65</v>
       </c>
-      <c r="K55" t="n">
+      <c r="L55" t="n">
         <v>0.002570656580342945</v>
       </c>
-      <c r="L55" t="n">
+      <c r="M55" t="n">
         <v>24.1770251381254</v>
       </c>
     </row>
@@ -2561,27 +2728,30 @@
         <v>3562.5</v>
       </c>
       <c r="E56" t="n">
-        <v>106406</v>
+        <v>4227.5</v>
       </c>
       <c r="F56" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G56" t="n">
         <v>266.9269563007828</v>
       </c>
-      <c r="G56" t="n">
+      <c r="H56" t="n">
         <v>0.07492686492653551</v>
       </c>
-      <c r="H56" t="n">
+      <c r="I56" t="n">
         <v>2.247805947796065</v>
       </c>
-      <c r="I56" t="n">
+      <c r="J56" t="n">
         <v>53.94734274710557</v>
       </c>
-      <c r="J56" t="n">
+      <c r="K56" t="n">
         <v>40</v>
       </c>
-      <c r="K56" t="n">
+      <c r="L56" t="n">
         <v>0.00292540293857968</v>
       </c>
-      <c r="L56" t="n">
+      <c r="M56" t="n">
         <v>10.42174796869011</v>
       </c>
     </row>
@@ -2599,27 +2769,30 @@
         <v>5700</v>
       </c>
       <c r="E57" t="n">
-        <v>106406</v>
+        <v>2683.75</v>
       </c>
       <c r="F57" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G57" t="n">
         <v>337.6388603226827</v>
       </c>
-      <c r="G57" t="n">
+      <c r="H57" t="n">
         <v>0.05923488777590924</v>
       </c>
-      <c r="H57" t="n">
+      <c r="I57" t="n">
         <v>1.777046633277277</v>
       </c>
-      <c r="I57" t="n">
+      <c r="J57" t="n">
         <v>42.64911919865465</v>
       </c>
-      <c r="J57" t="n">
+      <c r="K57" t="n">
         <v>50</v>
       </c>
-      <c r="K57" t="n">
+      <c r="L57" t="n">
         <v>0.03825561120453802</v>
       </c>
-      <c r="L57" t="n">
+      <c r="M57" t="n">
         <v>218.0569838658667</v>
       </c>
     </row>
@@ -2637,27 +2810,30 @@
         <v>6412.5</v>
       </c>
       <c r="E58" t="n">
-        <v>106406</v>
+        <v>1591.25</v>
       </c>
       <c r="F58" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G58" t="n">
         <v>358.1200915893996</v>
       </c>
-      <c r="G58" t="n">
+      <c r="H58" t="n">
         <v>0.05584718777222607</v>
       </c>
-      <c r="H58" t="n">
+      <c r="I58" t="n">
         <v>1.675415633166782</v>
       </c>
-      <c r="I58" t="n">
+      <c r="J58" t="n">
         <v>40.20997519600277</v>
       </c>
-      <c r="J58" t="n">
+      <c r="K58" t="n">
         <v>53</v>
       </c>
-      <c r="K58" t="n">
+      <c r="L58" t="n">
         <v>0.04009904807201847</v>
       </c>
-      <c r="L58" t="n">
+      <c r="M58" t="n">
         <v>257.1351457618185</v>
       </c>
     </row>
@@ -2675,27 +2851,30 @@
         <v>5415</v>
       </c>
       <c r="E59" t="n">
-        <v>106406</v>
+        <v>2018.75</v>
       </c>
       <c r="F59" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G59" t="n">
         <v>329.0896534380867</v>
       </c>
-      <c r="G59" t="n">
+      <c r="H59" t="n">
         <v>0.0607737125462764</v>
       </c>
-      <c r="H59" t="n">
+      <c r="I59" t="n">
         <v>1.823211376388292</v>
       </c>
-      <c r="I59" t="n">
+      <c r="J59" t="n">
         <v>43.75707303331901</v>
       </c>
-      <c r="J59" t="n">
+      <c r="K59" t="n">
         <v>49</v>
       </c>
-      <c r="K59" t="n">
+      <c r="L59" t="n">
         <v>0.02208808523245631</v>
       </c>
-      <c r="L59" t="n">
+      <c r="M59" t="n">
         <v>119.6069815337509</v>
       </c>
     </row>
@@ -2713,27 +2892,30 @@
         <v>3277.5</v>
       </c>
       <c r="E60" t="n">
-        <v>106406</v>
+        <v>1947.5</v>
       </c>
       <c r="F60" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G60" t="n">
         <v>256.0273422898422</v>
       </c>
-      <c r="G60" t="n">
+      <c r="H60" t="n">
         <v>0.07811665668645071</v>
       </c>
-      <c r="H60" t="n">
+      <c r="I60" t="n">
         <v>2.343499700593521</v>
       </c>
-      <c r="I60" t="n">
+      <c r="J60" t="n">
         <v>56.24399281424451</v>
       </c>
-      <c r="J60" t="n">
+      <c r="K60" t="n">
         <v>38</v>
       </c>
-      <c r="K60" t="n">
+      <c r="L60" t="n">
         <v>0.03156704591487314</v>
       </c>
-      <c r="L60" t="n">
+      <c r="M60" t="n">
         <v>103.4609929859967</v>
       </c>
     </row>
@@ -2751,27 +2933,30 @@
         <v>3847.5</v>
       </c>
       <c r="E61" t="n">
-        <v>106406</v>
+        <v>2232.5</v>
       </c>
       <c r="F61" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G61" t="n">
         <v>277.3986301336039</v>
       </c>
-      <c r="G61" t="n">
+      <c r="H61" t="n">
         <v>0.07209840939145001</v>
       </c>
-      <c r="H61" t="n">
+      <c r="I61" t="n">
         <v>2.1629522817435</v>
       </c>
-      <c r="I61" t="n">
+      <c r="J61" t="n">
         <v>51.91085476184401</v>
       </c>
-      <c r="J61" t="n">
+      <c r="K61" t="n">
         <v>41</v>
       </c>
-      <c r="K61" t="n">
+      <c r="L61" t="n">
         <v>0.04396521495054939</v>
       </c>
-      <c r="L61" t="n">
+      <c r="M61" t="n">
         <v>169.1561645222388</v>
       </c>
     </row>
@@ -2789,27 +2974,30 @@
         <v>9690</v>
       </c>
       <c r="E62" t="n">
-        <v>106406</v>
+        <v>2280</v>
       </c>
       <c r="F62" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G62" t="n">
         <v>440.2272140611028</v>
       </c>
-      <c r="G62" t="n">
+      <c r="H62" t="n">
         <v>0.04543108504242546</v>
       </c>
-      <c r="H62" t="n">
+      <c r="I62" t="n">
         <v>1.362932551272764</v>
       </c>
-      <c r="I62" t="n">
+      <c r="J62" t="n">
         <v>32.71038123054633</v>
       </c>
-      <c r="J62" t="n">
+      <c r="K62" t="n">
         <v>66</v>
       </c>
-      <c r="K62" t="n">
+      <c r="L62" t="n">
         <v>0.001548387199919343</v>
       </c>
-      <c r="L62" t="n">
+      <c r="M62" t="n">
         <v>15.00387196721844</v>
       </c>
     </row>
@@ -2827,27 +3015,30 @@
         <v>2137.5</v>
       </c>
       <c r="E63" t="n">
-        <v>106406</v>
+        <v>2470</v>
       </c>
       <c r="F63" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G63" t="n">
         <v>206.7607312813533</v>
       </c>
-      <c r="G63" t="n">
+      <c r="H63" t="n">
         <v>0.09673016668133488</v>
       </c>
-      <c r="H63" t="n">
+      <c r="I63" t="n">
         <v>2.901905000440046</v>
       </c>
-      <c r="I63" t="n">
+      <c r="J63" t="n">
         <v>69.64572001056112</v>
       </c>
-      <c r="J63" t="n">
+      <c r="K63" t="n">
         <v>31</v>
       </c>
-      <c r="K63" t="n">
+      <c r="L63" t="n">
         <v>0.00136483287861866</v>
       </c>
-      <c r="L63" t="n">
+      <c r="M63" t="n">
         <v>2.917330278047387</v>
       </c>
     </row>
@@ -2865,27 +3056,30 @@
         <v>2707.5</v>
       </c>
       <c r="E64" t="n">
-        <v>106406</v>
+        <v>3467.5</v>
       </c>
       <c r="F64" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G64" t="n">
         <v>232.7015255644019</v>
       </c>
-      <c r="G64" t="n">
+      <c r="H64" t="n">
         <v>0.085947008518708</v>
       </c>
-      <c r="H64" t="n">
+      <c r="I64" t="n">
         <v>2.57841025556124</v>
       </c>
-      <c r="I64" t="n">
+      <c r="J64" t="n">
         <v>61.88184613346976</v>
       </c>
-      <c r="J64" t="n">
+      <c r="K64" t="n">
         <v>34</v>
       </c>
-      <c r="K64" t="n">
+      <c r="L64" t="n">
         <v>0.07780171036392813</v>
       </c>
-      <c r="L64" t="n">
+      <c r="M64" t="n">
         <v>210.6481308103354</v>
       </c>
     </row>
@@ -2903,27 +3097,30 @@
         <v>1852.5</v>
       </c>
       <c r="E65" t="n">
-        <v>106406</v>
+        <v>3325</v>
       </c>
       <c r="F65" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G65" t="n">
         <v>192.4837655492016</v>
       </c>
-      <c r="G65" t="n">
+      <c r="H65" t="n">
         <v>0.1039048666932262</v>
       </c>
-      <c r="H65" t="n">
+      <c r="I65" t="n">
         <v>3.117146000796786</v>
       </c>
-      <c r="I65" t="n">
+      <c r="J65" t="n">
         <v>74.81150401912286</v>
       </c>
-      <c r="J65" t="n">
+      <c r="K65" t="n">
         <v>28</v>
       </c>
-      <c r="K65" t="n">
+      <c r="L65" t="n">
         <v>0.09066373258966598</v>
       </c>
-      <c r="L65" t="n">
+      <c r="M65" t="n">
         <v>167.9545646223562</v>
       </c>
     </row>
@@ -2941,27 +3138,30 @@
         <v>4417.5</v>
       </c>
       <c r="E66" t="n">
-        <v>106406</v>
+        <v>3040</v>
       </c>
       <c r="F66" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G66" t="n">
         <v>297.237278954037</v>
       </c>
-      <c r="G66" t="n">
+      <c r="H66" t="n">
         <v>0.06728631102524889</v>
       </c>
-      <c r="H66" t="n">
+      <c r="I66" t="n">
         <v>2.018589330757467</v>
       </c>
-      <c r="I66" t="n">
+      <c r="J66" t="n">
         <v>48.4461439381792</v>
       </c>
-      <c r="J66" t="n">
+      <c r="K66" t="n">
         <v>44</v>
       </c>
-      <c r="K66" t="n">
+      <c r="L66" t="n">
         <v>0.03940231488904899</v>
       </c>
-      <c r="L66" t="n">
+      <c r="M66" t="n">
         <v>174.0597260223739</v>
       </c>
     </row>
@@ -2979,27 +3179,30 @@
         <v>2280</v>
       </c>
       <c r="E67" t="n">
-        <v>106406</v>
+        <v>2232.5</v>
       </c>
       <c r="F67" t="n">
+        <v>106406</v>
+      </c>
+      <c r="G67" t="n">
         <v>213.5415650406262</v>
       </c>
-      <c r="G67" t="n">
+      <c r="H67" t="n">
         <v>0.09365858115816939</v>
       </c>
-      <c r="H67" t="n">
+      <c r="I67" t="n">
         <v>2.809757434745082</v>
       </c>
-      <c r="I67" t="n">
+      <c r="J67" t="n">
         <v>67.43417843388195</v>
       </c>
-      <c r="J67" t="n">
+      <c r="K67" t="n">
         <v>32</v>
       </c>
-      <c r="K67" t="n">
+      <c r="L67" t="n">
         <v>0.00292540293857968</v>
       </c>
-      <c r="L67" t="n">
+      <c r="M67" t="n">
         <v>6.66991869996167</v>
       </c>
     </row>
@@ -3017,27 +3220,30 @@
         <v>4275</v>
       </c>
       <c r="E68" t="n">
+        <v>2565</v>
+      </c>
+      <c r="F68" t="n">
         <v>106968</v>
       </c>
-      <c r="F68" t="n">
+      <c r="G68" t="n">
         <v>292.4038303442689</v>
       </c>
-      <c r="G68" t="n">
+      <c r="H68" t="n">
         <v>0.06839855680567694</v>
       </c>
-      <c r="H68" t="n">
+      <c r="I68" t="n">
         <v>2.051956704170308</v>
       </c>
-      <c r="I68" t="n">
+      <c r="J68" t="n">
         <v>49.2469609000874</v>
       </c>
-      <c r="J68" t="n">
+      <c r="K68" t="n">
         <v>29</v>
       </c>
-      <c r="K68" t="n">
+      <c r="L68" t="n">
         <v>0.01644185263536868</v>
       </c>
-      <c r="L68" t="n">
+      <c r="M68" t="n">
         <v>70.28892001620112</v>
       </c>
     </row>
@@ -3055,27 +3261,30 @@
         <v>10402.5</v>
       </c>
       <c r="E69" t="n">
+        <v>2802.5</v>
+      </c>
+      <c r="F69" t="n">
         <v>106968</v>
       </c>
-      <c r="F69" t="n">
+      <c r="G69" t="n">
         <v>456.1249828720194</v>
       </c>
-      <c r="G69" t="n">
+      <c r="H69" t="n">
         <v>0.04384763113405618</v>
       </c>
-      <c r="H69" t="n">
+      <c r="I69" t="n">
         <v>1.315428934021685</v>
       </c>
-      <c r="I69" t="n">
+      <c r="J69" t="n">
         <v>31.57029441652045</v>
       </c>
-      <c r="J69" t="n">
+      <c r="K69" t="n">
         <v>45</v>
       </c>
-      <c r="K69" t="n">
+      <c r="L69" t="n">
         <v>0.02685659896747183</v>
       </c>
-      <c r="L69" t="n">
+      <c r="M69" t="n">
         <v>279.3757707591258</v>
       </c>
     </row>
@@ -3093,27 +3302,30 @@
         <v>4132.5</v>
       </c>
       <c r="E70" t="n">
+        <v>3325</v>
+      </c>
+      <c r="F70" t="n">
         <v>106968</v>
       </c>
-      <c r="F70" t="n">
+      <c r="G70" t="n">
         <v>287.489130229301</v>
       </c>
-      <c r="G70" t="n">
+      <c r="H70" t="n">
         <v>0.06956784760539649</v>
       </c>
-      <c r="H70" t="n">
+      <c r="I70" t="n">
         <v>2.087035428161895</v>
       </c>
-      <c r="I70" t="n">
+      <c r="J70" t="n">
         <v>50.08885027588547</v>
       </c>
-      <c r="J70" t="n">
+      <c r="K70" t="n">
         <v>28</v>
       </c>
-      <c r="K70" t="n">
+      <c r="L70" t="n">
         <v>0.05210026704889836</v>
       </c>
-      <c r="L70" t="n">
+      <c r="M70" t="n">
         <v>215.3043535795725</v>
       </c>
     </row>
@@ -3131,27 +3343,30 @@
         <v>5985</v>
       </c>
       <c r="E71" t="n">
+        <v>3230</v>
+      </c>
+      <c r="F71" t="n">
         <v>106968</v>
       </c>
-      <c r="F71" t="n">
+      <c r="G71" t="n">
         <v>345.9768778401239</v>
       </c>
-      <c r="G71" t="n">
+      <c r="H71" t="n">
         <v>0.05780733130160801</v>
       </c>
-      <c r="H71" t="n">
+      <c r="I71" t="n">
         <v>1.73421993904824</v>
       </c>
-      <c r="I71" t="n">
+      <c r="J71" t="n">
         <v>41.62127853715776</v>
       </c>
-      <c r="J71" t="n">
+      <c r="K71" t="n">
         <v>34</v>
       </c>
-      <c r="K71" t="n">
+      <c r="L71" t="n">
         <v>0.03455073574532785</v>
       </c>
-      <c r="L71" t="n">
+      <c r="M71" t="n">
         <v>206.7861534357872</v>
       </c>
     </row>
@@ -3169,27 +3384,30 @@
         <v>11257.5</v>
       </c>
       <c r="E72" t="n">
+        <v>2945</v>
+      </c>
+      <c r="F72" t="n">
         <v>106968</v>
       </c>
-      <c r="F72" t="n">
+      <c r="G72" t="n">
         <v>474.4997365647319</v>
       </c>
-      <c r="G72" t="n">
+      <c r="H72" t="n">
         <v>0.04214965459158178</v>
       </c>
-      <c r="H72" t="n">
+      <c r="I72" t="n">
         <v>1.264489637747453</v>
       </c>
-      <c r="I72" t="n">
+      <c r="J72" t="n">
         <v>30.34775130593888</v>
       </c>
-      <c r="J72" t="n">
+      <c r="K72" t="n">
         <v>47</v>
       </c>
-      <c r="K72" t="n">
+      <c r="L72" t="n">
         <v>0.01896623419565646</v>
       </c>
-      <c r="L72" t="n">
+      <c r="M72" t="n">
         <v>213.5123814576026</v>
       </c>
     </row>
@@ -3207,27 +3425,30 @@
         <v>5842.5</v>
       </c>
       <c r="E73" t="n">
+        <v>2185</v>
+      </c>
+      <c r="F73" t="n">
         <v>106968</v>
       </c>
-      <c r="F73" t="n">
+      <c r="G73" t="n">
         <v>341.8332927027442</v>
       </c>
-      <c r="G73" t="n">
+      <c r="H73" t="n">
         <v>0.05850805181048253</v>
       </c>
-      <c r="H73" t="n">
+      <c r="I73" t="n">
         <v>1.755241554314476</v>
       </c>
-      <c r="I73" t="n">
+      <c r="J73" t="n">
         <v>42.12579730354742</v>
       </c>
-      <c r="J73" t="n">
+      <c r="K73" t="n">
         <v>34</v>
       </c>
-      <c r="K73" t="n">
+      <c r="L73" t="n">
         <v>0.01072623844359377</v>
       </c>
-      <c r="L73" t="n">
+      <c r="M73" t="n">
         <v>62.66804810669661</v>
       </c>
     </row>
@@ -3245,27 +3466,30 @@
         <v>11400</v>
       </c>
       <c r="E74" t="n">
+        <v>2612.5</v>
+      </c>
+      <c r="F74" t="n">
         <v>106968</v>
       </c>
-      <c r="F74" t="n">
+      <c r="G74" t="n">
         <v>477.4934554525329</v>
       </c>
-      <c r="G74" t="n">
+      <c r="H74" t="n">
         <v>0.04188539082916955</v>
       </c>
-      <c r="H74" t="n">
+      <c r="I74" t="n">
         <v>1.256561724875087</v>
       </c>
-      <c r="I74" t="n">
+      <c r="J74" t="n">
         <v>30.15748139700208</v>
       </c>
-      <c r="J74" t="n">
+      <c r="K74" t="n">
         <v>47</v>
       </c>
-      <c r="K74" t="n">
+      <c r="L74" t="n">
         <v>0.03138663102903094</v>
       </c>
-      <c r="L74" t="n">
+      <c r="M74" t="n">
         <v>357.8075937309528</v>
       </c>
     </row>
@@ -3283,27 +3507,30 @@
         <v>10545</v>
       </c>
       <c r="E75" t="n">
+        <v>3562.5</v>
+      </c>
+      <c r="F75" t="n">
         <v>106968</v>
       </c>
-      <c r="F75" t="n">
+      <c r="G75" t="n">
         <v>459.2385001282013</v>
       </c>
-      <c r="G75" t="n">
+      <c r="H75" t="n">
         <v>0.04355035563093422</v>
       </c>
-      <c r="H75" t="n">
+      <c r="I75" t="n">
         <v>1.306510668928027</v>
       </c>
-      <c r="I75" t="n">
+      <c r="J75" t="n">
         <v>31.35625605427264</v>
       </c>
-      <c r="J75" t="n">
+      <c r="K75" t="n">
         <v>45</v>
       </c>
-      <c r="K75" t="n">
+      <c r="L75" t="n">
         <v>0.04023399660796012</v>
       </c>
-      <c r="L75" t="n">
+      <c r="M75" t="n">
         <v>424.2674942309395</v>
       </c>
     </row>
@@ -3321,27 +3548,30 @@
         <v>15532.5</v>
       </c>
       <c r="E76" t="n">
+        <v>4417.5</v>
+      </c>
+      <c r="F76" t="n">
         <v>106968</v>
       </c>
-      <c r="F76" t="n">
+      <c r="G76" t="n">
         <v>557.3598478541489</v>
       </c>
-      <c r="G76" t="n">
+      <c r="H76" t="n">
         <v>0.03588346034792525</v>
       </c>
-      <c r="H76" t="n">
+      <c r="I76" t="n">
         <v>1.076503810437758</v>
       </c>
-      <c r="I76" t="n">
+      <c r="J76" t="n">
         <v>25.83609145050618</v>
       </c>
-      <c r="J76" t="n">
+      <c r="K76" t="n">
         <v>55</v>
       </c>
-      <c r="K76" t="n">
+      <c r="L76" t="n">
         <v>0.02640968086411122</v>
       </c>
-      <c r="L76" t="n">
+      <c r="M76" t="n">
         <v>410.2083680218075</v>
       </c>
     </row>
@@ -3359,27 +3589,30 @@
         <v>10402.5</v>
       </c>
       <c r="E77" t="n">
+        <v>3847.5</v>
+      </c>
+      <c r="F77" t="n">
         <v>106968</v>
       </c>
-      <c r="F77" t="n">
+      <c r="G77" t="n">
         <v>456.1249828720194</v>
       </c>
-      <c r="G77" t="n">
+      <c r="H77" t="n">
         <v>0.04384763113405618</v>
       </c>
-      <c r="H77" t="n">
+      <c r="I77" t="n">
         <v>1.315428934021685</v>
       </c>
-      <c r="I77" t="n">
+      <c r="J77" t="n">
         <v>31.57029441652045</v>
       </c>
-      <c r="J77" t="n">
+      <c r="K77" t="n">
         <v>45</v>
       </c>
-      <c r="K77" t="n">
+      <c r="L77" t="n">
         <v>0.02685659896747183</v>
       </c>
-      <c r="L77" t="n">
+      <c r="M77" t="n">
         <v>279.3757707591258</v>
       </c>
     </row>
@@ -3397,27 +3630,30 @@
         <v>13680</v>
       </c>
       <c r="E78" t="n">
+        <v>3420</v>
+      </c>
+      <c r="F78" t="n">
         <v>106968</v>
       </c>
-      <c r="F78" t="n">
+      <c r="G78" t="n">
         <v>523.0678732248808</v>
       </c>
-      <c r="G78" t="n">
+      <c r="H78" t="n">
         <v>0.03823595564509363</v>
       </c>
-      <c r="H78" t="n">
+      <c r="I78" t="n">
         <v>1.147078669352809</v>
       </c>
-      <c r="I78" t="n">
+      <c r="J78" t="n">
         <v>27.52988806446741</v>
       </c>
-      <c r="J78" t="n">
+      <c r="K78" t="n">
         <v>52</v>
       </c>
-      <c r="K78" t="n">
+      <c r="L78" t="n">
         <v>0.01173030645513151</v>
       </c>
-      <c r="L78" t="n">
+      <c r="M78" t="n">
         <v>160.4705923061991</v>
       </c>
     </row>
@@ -3435,27 +3671,30 @@
         <v>8835</v>
       </c>
       <c r="E79" t="n">
+        <v>2565</v>
+      </c>
+      <c r="F79" t="n">
         <v>106968</v>
       </c>
-      <c r="F79" t="n">
+      <c r="G79" t="n">
         <v>420.3569911396741</v>
       </c>
-      <c r="G79" t="n">
+      <c r="H79" t="n">
         <v>0.04757860680698065</v>
       </c>
-      <c r="H79" t="n">
+      <c r="I79" t="n">
         <v>1.42735820420942</v>
       </c>
-      <c r="I79" t="n">
+      <c r="J79" t="n">
         <v>34.25659690102607</v>
       </c>
-      <c r="J79" t="n">
+      <c r="K79" t="n">
         <v>42</v>
       </c>
-      <c r="K79" t="n">
+      <c r="L79" t="n">
         <v>0.001698514106812654</v>
       </c>
-      <c r="L79" t="n">
+      <c r="M79" t="n">
         <v>15.0063721336898</v>
       </c>
     </row>
@@ -3473,27 +3712,30 @@
         <v>11400</v>
       </c>
       <c r="E80" t="n">
+        <v>2945</v>
+      </c>
+      <c r="F80" t="n">
         <v>106968</v>
       </c>
-      <c r="F80" t="n">
+      <c r="G80" t="n">
         <v>477.4934554525329</v>
       </c>
-      <c r="G80" t="n">
+      <c r="H80" t="n">
         <v>0.04188539082916955</v>
       </c>
-      <c r="H80" t="n">
+      <c r="I80" t="n">
         <v>1.256561724875087</v>
       </c>
-      <c r="I80" t="n">
+      <c r="J80" t="n">
         <v>30.15748139700208</v>
       </c>
-      <c r="J80" t="n">
+      <c r="K80" t="n">
         <v>47</v>
       </c>
-      <c r="K80" t="n">
+      <c r="L80" t="n">
         <v>0.03138663102903094</v>
       </c>
-      <c r="L80" t="n">
+      <c r="M80" t="n">
         <v>357.8075937309528</v>
       </c>
     </row>
@@ -3511,27 +3753,30 @@
         <v>9832.5</v>
       </c>
       <c r="E81" t="n">
+        <v>3895</v>
+      </c>
+      <c r="F81" t="n">
         <v>106968</v>
       </c>
-      <c r="F81" t="n">
+      <c r="G81" t="n">
         <v>443.4523649728345</v>
       </c>
-      <c r="G81" t="n">
+      <c r="H81" t="n">
         <v>0.04510067276611589</v>
       </c>
-      <c r="H81" t="n">
+      <c r="I81" t="n">
         <v>1.353020182983477</v>
       </c>
-      <c r="I81" t="n">
+      <c r="J81" t="n">
         <v>32.47248439160344</v>
       </c>
-      <c r="J81" t="n">
+      <c r="K81" t="n">
         <v>44</v>
       </c>
-      <c r="K81" t="n">
+      <c r="L81" t="n">
         <v>0.01557039829090101</v>
       </c>
-      <c r="L81" t="n">
+      <c r="M81" t="n">
         <v>153.0959411952842</v>
       </c>
     </row>
@@ -3549,27 +3794,30 @@
         <v>6982.5</v>
       </c>
       <c r="E82" t="n">
+        <v>4322.5</v>
+      </c>
+      <c r="F82" t="n">
         <v>106968</v>
       </c>
-      <c r="F82" t="n">
+      <c r="G82" t="n">
         <v>373.6977388210959</v>
       </c>
-      <c r="G82" t="n">
+      <c r="H82" t="n">
         <v>0.05351918923323965</v>
       </c>
-      <c r="H82" t="n">
+      <c r="I82" t="n">
         <v>1.60557567699719</v>
       </c>
-      <c r="I82" t="n">
+      <c r="J82" t="n">
         <v>38.53381624793255</v>
       </c>
-      <c r="J82" t="n">
+      <c r="K82" t="n">
         <v>37</v>
       </c>
-      <c r="K82" t="n">
+      <c r="L82" t="n">
         <v>0.01978999837013284</v>
       </c>
-      <c r="L82" t="n">
+      <c r="M82" t="n">
         <v>138.1836636194526</v>
       </c>
     </row>
@@ -3587,27 +3835,30 @@
         <v>12255</v>
       </c>
       <c r="E83" t="n">
+        <v>5130</v>
+      </c>
+      <c r="F83" t="n">
         <v>106968</v>
       </c>
-      <c r="F83" t="n">
+      <c r="G83" t="n">
         <v>495.0757517794625</v>
       </c>
-      <c r="G83" t="n">
+      <c r="H83" t="n">
         <v>0.04039785816233884</v>
       </c>
-      <c r="H83" t="n">
+      <c r="I83" t="n">
         <v>1.211935744870165</v>
       </c>
-      <c r="I83" t="n">
+      <c r="J83" t="n">
         <v>29.08645787688396</v>
       </c>
-      <c r="J83" t="n">
+      <c r="K83" t="n">
         <v>49</v>
       </c>
-      <c r="K83" t="n">
+      <c r="L83" t="n">
         <v>0.02050495004539687</v>
       </c>
-      <c r="L83" t="n">
+      <c r="M83" t="n">
         <v>251.2881628063387</v>
       </c>
     </row>
@@ -3625,27 +3876,30 @@
         <v>5557.5</v>
       </c>
       <c r="E84" t="n">
+        <v>5225</v>
+      </c>
+      <c r="F84" t="n">
         <v>106968</v>
       </c>
-      <c r="F84" t="n">
+      <c r="G84" t="n">
         <v>333.391661563393</v>
       </c>
-      <c r="G84" t="n">
+      <c r="H84" t="n">
         <v>0.05998950275544634</v>
       </c>
-      <c r="H84" t="n">
+      <c r="I84" t="n">
         <v>1.79968508266339</v>
       </c>
-      <c r="I84" t="n">
+      <c r="J84" t="n">
         <v>43.19244198392136</v>
       </c>
-      <c r="J84" t="n">
+      <c r="K84" t="n">
         <v>33</v>
       </c>
-      <c r="K84" t="n">
+      <c r="L84" t="n">
         <v>0.02034640907027097</v>
       </c>
-      <c r="L84" t="n">
+      <c r="M84" t="n">
         <v>113.0751684080309</v>
       </c>
     </row>
@@ -3663,27 +3917,30 @@
         <v>7980</v>
       </c>
       <c r="E85" t="n">
+        <v>5842.5</v>
+      </c>
+      <c r="F85" t="n">
         <v>106968</v>
       </c>
-      <c r="F85" t="n">
+      <c r="G85" t="n">
         <v>399.4996871087636</v>
       </c>
-      <c r="G85" t="n">
+      <c r="H85" t="n">
         <v>0.05006261743217588</v>
       </c>
-      <c r="H85" t="n">
+      <c r="I85" t="n">
         <v>1.501878522965276</v>
       </c>
-      <c r="I85" t="n">
+      <c r="J85" t="n">
         <v>36.04508455116664</v>
       </c>
-      <c r="J85" t="n">
+      <c r="K85" t="n">
         <v>39</v>
       </c>
-      <c r="K85" t="n">
+      <c r="L85" t="n">
         <v>0.0475579201451406</v>
       </c>
-      <c r="L85" t="n">
+      <c r="M85" t="n">
         <v>379.512202758222</v>
       </c>
     </row>
@@ -3701,27 +3958,30 @@
         <v>8265</v>
       </c>
       <c r="E86" t="n">
+        <v>5035</v>
+      </c>
+      <c r="F86" t="n">
         <v>106968</v>
       </c>
-      <c r="F86" t="n">
+      <c r="G86" t="n">
         <v>406.5710270051225</v>
       </c>
-      <c r="G86" t="n">
+      <c r="H86" t="n">
         <v>0.04919189679432819</v>
       </c>
-      <c r="H86" t="n">
+      <c r="I86" t="n">
         <v>1.475756903829845</v>
       </c>
-      <c r="I86" t="n">
+      <c r="J86" t="n">
         <v>35.41816569191629</v>
       </c>
-      <c r="J86" t="n">
+      <c r="K86" t="n">
         <v>40</v>
       </c>
-      <c r="K86" t="n">
+      <c r="L86" t="n">
         <v>0.03232412822687269</v>
       </c>
-      <c r="L86" t="n">
+      <c r="M86" t="n">
         <v>267.1589197951028</v>
       </c>
     </row>
@@ -3739,27 +3999,30 @@
         <v>10260</v>
       </c>
       <c r="E87" t="n">
+        <v>4180</v>
+      </c>
+      <c r="F87" t="n">
         <v>106968</v>
       </c>
-      <c r="F87" t="n">
+      <c r="G87" t="n">
         <v>452.990066116245</v>
       </c>
-      <c r="G87" t="n">
+      <c r="H87" t="n">
         <v>0.0441510785688348</v>
       </c>
-      <c r="H87" t="n">
+      <c r="I87" t="n">
         <v>1.324532357065044</v>
       </c>
-      <c r="I87" t="n">
+      <c r="J87" t="n">
         <v>31.78877656956105</v>
       </c>
-      <c r="J87" t="n">
+      <c r="K87" t="n">
         <v>45</v>
       </c>
-      <c r="K87" t="n">
+      <c r="L87" t="n">
         <v>0.0132014644024343</v>
       </c>
-      <c r="L87" t="n">
+      <c r="M87" t="n">
         <v>135.447024768976</v>
       </c>
     </row>
@@ -3777,27 +4040,30 @@
         <v>10545</v>
       </c>
       <c r="E88" t="n">
+        <v>5605</v>
+      </c>
+      <c r="F88" t="n">
         <v>106968</v>
       </c>
-      <c r="F88" t="n">
+      <c r="G88" t="n">
         <v>459.2385001282013</v>
       </c>
-      <c r="G88" t="n">
+      <c r="H88" t="n">
         <v>0.04355035563093422</v>
       </c>
-      <c r="H88" t="n">
+      <c r="I88" t="n">
         <v>1.306510668928027</v>
       </c>
-      <c r="I88" t="n">
+      <c r="J88" t="n">
         <v>31.35625605427264</v>
       </c>
-      <c r="J88" t="n">
+      <c r="K88" t="n">
         <v>45</v>
       </c>
-      <c r="K88" t="n">
+      <c r="L88" t="n">
         <v>0.04023399660796012</v>
       </c>
-      <c r="L88" t="n">
+      <c r="M88" t="n">
         <v>424.2674942309395</v>
       </c>
     </row>
@@ -3815,27 +4081,30 @@
         <v>14677.5</v>
       </c>
       <c r="E89" t="n">
+        <v>5225</v>
+      </c>
+      <c r="F89" t="n">
         <v>106968</v>
       </c>
-      <c r="F89" t="n">
+      <c r="G89" t="n">
         <v>541.8025470593508</v>
       </c>
-      <c r="G89" t="n">
+      <c r="H89" t="n">
         <v>0.03691381686658837</v>
       </c>
-      <c r="H89" t="n">
+      <c r="I89" t="n">
         <v>1.107414505997651</v>
       </c>
-      <c r="I89" t="n">
+      <c r="J89" t="n">
         <v>26.57794814394362</v>
       </c>
-      <c r="J89" t="n">
+      <c r="K89" t="n">
         <v>54</v>
       </c>
-      <c r="K89" t="n">
+      <c r="L89" t="n">
         <v>0.006653889204228269</v>
       </c>
-      <c r="L89" t="n">
+      <c r="M89" t="n">
         <v>97.66245879506042</v>
       </c>
     </row>
@@ -3853,27 +4122,30 @@
         <v>11115</v>
       </c>
       <c r="E90" t="n">
+        <v>4845</v>
+      </c>
+      <c r="F90" t="n">
         <v>106968</v>
       </c>
-      <c r="F90" t="n">
+      <c r="G90" t="n">
         <v>471.4870093650513</v>
       </c>
-      <c r="G90" t="n">
+      <c r="H90" t="n">
         <v>0.04241898419838518</v>
       </c>
-      <c r="H90" t="n">
+      <c r="I90" t="n">
         <v>1.272569525951555</v>
       </c>
-      <c r="I90" t="n">
+      <c r="J90" t="n">
         <v>30.54166862283733</v>
       </c>
-      <c r="J90" t="n">
+      <c r="K90" t="n">
         <v>47</v>
       </c>
-      <c r="K90" t="n">
+      <c r="L90" t="n">
         <v>0.006307742675896399</v>
       </c>
-      <c r="L90" t="n">
+      <c r="M90" t="n">
         <v>70.11055984258849</v>
       </c>
     </row>
@@ -3891,27 +4163,30 @@
         <v>11400</v>
       </c>
       <c r="E91" t="n">
+        <v>2232.5</v>
+      </c>
+      <c r="F91" t="n">
         <v>106968</v>
       </c>
-      <c r="F91" t="n">
+      <c r="G91" t="n">
         <v>477.4934554525329</v>
       </c>
-      <c r="G91" t="n">
+      <c r="H91" t="n">
         <v>0.04188539082916955</v>
       </c>
-      <c r="H91" t="n">
+      <c r="I91" t="n">
         <v>1.256561724875087</v>
       </c>
-      <c r="I91" t="n">
+      <c r="J91" t="n">
         <v>30.15748139700208</v>
       </c>
-      <c r="J91" t="n">
+      <c r="K91" t="n">
         <v>47</v>
       </c>
-      <c r="K91" t="n">
+      <c r="L91" t="n">
         <v>0.03138663102903094</v>
       </c>
-      <c r="L91" t="n">
+      <c r="M91" t="n">
         <v>357.8075937309528</v>
       </c>
     </row>
@@ -3929,27 +4204,30 @@
         <v>12967.5</v>
       </c>
       <c r="E92" t="n">
+        <v>2992.5</v>
+      </c>
+      <c r="F92" t="n">
         <v>106968</v>
       </c>
-      <c r="F92" t="n">
+      <c r="G92" t="n">
         <v>509.2641750604494</v>
       </c>
-      <c r="G92" t="n">
+      <c r="H92" t="n">
         <v>0.03927234818279925</v>
       </c>
-      <c r="H92" t="n">
+      <c r="I92" t="n">
         <v>1.178170445483978</v>
       </c>
-      <c r="I92" t="n">
+      <c r="J92" t="n">
         <v>28.27609069161547</v>
       </c>
-      <c r="J92" t="n">
+      <c r="K92" t="n">
         <v>50</v>
       </c>
-      <c r="K92" t="n">
+      <c r="L92" t="n">
         <v>0.03638259086003726</v>
       </c>
-      <c r="L92" t="n">
+      <c r="M92" t="n">
         <v>471.7912469775331</v>
       </c>
     </row>
@@ -3967,27 +4245,30 @@
         <v>15960</v>
       </c>
       <c r="E93" t="n">
+        <v>2850</v>
+      </c>
+      <c r="F93" t="n">
         <v>106968</v>
       </c>
-      <c r="F93" t="n">
+      <c r="G93" t="n">
         <v>564.9778756730213</v>
       </c>
-      <c r="G93" t="n">
+      <c r="H93" t="n">
         <v>0.03539961627023943</v>
       </c>
-      <c r="H93" t="n">
+      <c r="I93" t="n">
         <v>1.061988488107183</v>
       </c>
-      <c r="I93" t="n">
+      <c r="J93" t="n">
         <v>25.48772371457239</v>
       </c>
-      <c r="J93" t="n">
+      <c r="K93" t="n">
         <v>56</v>
       </c>
-      <c r="K93" t="n">
+      <c r="L93" t="n">
         <v>0.01762148886659198</v>
       </c>
-      <c r="L93" t="n">
+      <c r="M93" t="n">
         <v>281.2389623108081</v>
       </c>
     </row>
@@ -4005,27 +4286,30 @@
         <v>1995</v>
       </c>
       <c r="E94" t="n">
+        <v>3420</v>
+      </c>
+      <c r="F94" t="n">
         <v>106968</v>
       </c>
-      <c r="F94" t="n">
+      <c r="G94" t="n">
         <v>199.7498435543818</v>
       </c>
-      <c r="G94" t="n">
+      <c r="H94" t="n">
         <v>0.1001252348643518</v>
       </c>
-      <c r="H94" t="n">
+      <c r="I94" t="n">
         <v>3.003757045930553</v>
       </c>
-      <c r="I94" t="n">
+      <c r="J94" t="n">
         <v>72.09016910233328</v>
       </c>
-      <c r="J94" t="n">
+      <c r="K94" t="n">
         <v>19</v>
       </c>
-      <c r="K94" t="n">
+      <c r="L94" t="n">
         <v>0.09762053757731648</v>
       </c>
-      <c r="L94" t="n">
+      <c r="M94" t="n">
         <v>194.7529724667464</v>
       </c>
     </row>
@@ -4043,27 +4327,30 @@
         <v>8407.5</v>
       </c>
       <c r="E95" t="n">
+        <v>2137.5</v>
+      </c>
+      <c r="F95" t="n">
         <v>106968</v>
       </c>
-      <c r="F95" t="n">
+      <c r="G95" t="n">
         <v>410.0609710762535</v>
       </c>
-      <c r="G95" t="n">
+      <c r="H95" t="n">
         <v>0.04877323473996473</v>
       </c>
-      <c r="H95" t="n">
+      <c r="I95" t="n">
         <v>1.463197042198942</v>
       </c>
-      <c r="I95" t="n">
+      <c r="J95" t="n">
         <v>35.11672901277461</v>
       </c>
-      <c r="J95" t="n">
+      <c r="K95" t="n">
         <v>41</v>
       </c>
-      <c r="K95" t="n">
+      <c r="L95" t="n">
         <v>0.0002973756614459422</v>
       </c>
-      <c r="L95" t="n">
+      <c r="M95" t="n">
         <v>2.500185873606759</v>
       </c>
     </row>
@@ -4081,27 +4368,30 @@
         <v>7410</v>
       </c>
       <c r="E96" t="n">
+        <v>3040</v>
+      </c>
+      <c r="F96" t="n">
         <v>106968</v>
       </c>
-      <c r="F96" t="n">
+      <c r="G96" t="n">
         <v>384.9675310984031</v>
       </c>
-      <c r="G96" t="n">
+      <c r="H96" t="n">
         <v>0.05195243334661311</v>
       </c>
-      <c r="H96" t="n">
+      <c r="I96" t="n">
         <v>1.558573000398393</v>
       </c>
-      <c r="I96" t="n">
+      <c r="J96" t="n">
         <v>37.40575200956143</v>
       </c>
-      <c r="J96" t="n">
+      <c r="K96" t="n">
         <v>38</v>
       </c>
-      <c r="K96" t="n">
+      <c r="L96" t="n">
         <v>0.02580753282870196</v>
       </c>
-      <c r="L96" t="n">
+      <c r="M96" t="n">
         <v>191.2338182606815</v>
       </c>
     </row>
@@ -4119,27 +4409,30 @@
         <v>9120</v>
       </c>
       <c r="E97" t="n">
+        <v>2802.5</v>
+      </c>
+      <c r="F97" t="n">
         <v>106968</v>
       </c>
-      <c r="F97" t="n">
+      <c r="G97" t="n">
         <v>427.0831300812524</v>
       </c>
-      <c r="G97" t="n">
+      <c r="H97" t="n">
         <v>0.04682929057908469</v>
       </c>
-      <c r="H97" t="n">
+      <c r="I97" t="n">
         <v>1.404878717372541</v>
       </c>
-      <c r="I97" t="n">
+      <c r="J97" t="n">
         <v>33.71708921694098</v>
       </c>
-      <c r="J97" t="n">
+      <c r="K97" t="n">
         <v>42</v>
       </c>
-      <c r="K97" t="n">
+      <c r="L97" t="n">
         <v>0.03316979567844291</v>
       </c>
-      <c r="L97" t="n">
+      <c r="M97" t="n">
         <v>302.5085365873994</v>
       </c>
     </row>
@@ -4157,27 +4450,30 @@
         <v>6697.5</v>
       </c>
       <c r="E98" t="n">
+        <v>3467.5</v>
+      </c>
+      <c r="F98" t="n">
         <v>106968</v>
       </c>
-      <c r="F98" t="n">
+      <c r="G98" t="n">
         <v>365.991803186902</v>
       </c>
-      <c r="G98" t="n">
+      <c r="H98" t="n">
         <v>0.05464603257736498</v>
       </c>
-      <c r="H98" t="n">
+      <c r="I98" t="n">
         <v>1.639380977320949</v>
       </c>
-      <c r="I98" t="n">
+      <c r="J98" t="n">
         <v>39.34514345570278</v>
       </c>
-      <c r="J98" t="n">
+      <c r="K98" t="n">
         <v>36</v>
       </c>
-      <c r="K98" t="n">
+      <c r="L98" t="n">
         <v>0.03274282721486066</v>
       </c>
-      <c r="L98" t="n">
+      <c r="M98" t="n">
         <v>219.2950852715293</v>
       </c>
     </row>
@@ -4195,27 +4491,30 @@
         <v>17812.5</v>
       </c>
       <c r="E99" t="n">
+        <v>3040</v>
+      </c>
+      <c r="F99" t="n">
         <v>106968</v>
       </c>
-      <c r="F99" t="n">
+      <c r="G99" t="n">
         <v>596.8668193156661</v>
       </c>
-      <c r="G99" t="n">
+      <c r="H99" t="n">
         <v>0.03350831266333564</v>
       </c>
-      <c r="H99" t="n">
+      <c r="I99" t="n">
         <v>1.005249379900069</v>
       </c>
-      <c r="I99" t="n">
+      <c r="J99" t="n">
         <v>24.12598511760166</v>
       </c>
-      <c r="J99" t="n">
+      <c r="K99" t="n">
         <v>59</v>
       </c>
-      <c r="K99" t="n">
+      <c r="L99" t="n">
         <v>0.02300955286319706</v>
       </c>
-      <c r="L99" t="n">
+      <c r="M99" t="n">
         <v>409.8576603756976</v>
       </c>
     </row>
@@ -4233,27 +4532,30 @@
         <v>19665</v>
       </c>
       <c r="E100" t="n">
+        <v>2327.5</v>
+      </c>
+      <c r="F100" t="n">
         <v>106968</v>
       </c>
-      <c r="F100" t="n">
+      <c r="G100" t="n">
         <v>627.1363488110062</v>
       </c>
-      <c r="G100" t="n">
+      <c r="H100" t="n">
         <v>0.03189099154899599</v>
       </c>
-      <c r="H100" t="n">
+      <c r="I100" t="n">
         <v>0.9567297464698798</v>
       </c>
-      <c r="I100" t="n">
+      <c r="J100" t="n">
         <v>22.96151391527712</v>
       </c>
-      <c r="J100" t="n">
+      <c r="K100" t="n">
         <v>62</v>
       </c>
-      <c r="K100" t="n">
+      <c r="L100" t="n">
         <v>0.02275852396224831</v>
       </c>
-      <c r="L100" t="n">
+      <c r="M100" t="n">
         <v>447.5463737176131</v>
       </c>
     </row>
@@ -4271,27 +4573,30 @@
         <v>997.5</v>
       </c>
       <c r="E101" t="n">
+        <v>3372.5</v>
+      </c>
+      <c r="F101" t="n">
         <v>106968</v>
       </c>
-      <c r="F101" t="n">
+      <c r="G101" t="n">
         <v>141.2444689182553</v>
       </c>
-      <c r="G101" t="n">
+      <c r="H101" t="n">
         <v>0.1415984650809577</v>
       </c>
-      <c r="H101" t="n">
+      <c r="I101" t="n">
         <v>4.247953952428731</v>
       </c>
-      <c r="I101" t="n">
+      <c r="J101" t="n">
         <v>101.9508948582896</v>
       </c>
-      <c r="J101" t="n">
+      <c r="K101" t="n">
         <v>14</v>
       </c>
-      <c r="K101" t="n">
+      <c r="L101" t="n">
         <v>0.01762148886659198</v>
       </c>
-      <c r="L101" t="n">
+      <c r="M101" t="n">
         <v>17.5774351444255</v>
       </c>
     </row>
@@ -4309,27 +4614,30 @@
         <v>6982.5</v>
       </c>
       <c r="E102" t="n">
+        <v>4607.5</v>
+      </c>
+      <c r="F102" t="n">
         <v>106968</v>
       </c>
-      <c r="F102" t="n">
+      <c r="G102" t="n">
         <v>373.6977388210959</v>
       </c>
-      <c r="G102" t="n">
+      <c r="H102" t="n">
         <v>0.05351918923323965</v>
       </c>
-      <c r="H102" t="n">
+      <c r="I102" t="n">
         <v>1.60557567699719</v>
       </c>
-      <c r="I102" t="n">
+      <c r="J102" t="n">
         <v>38.53381624793255</v>
       </c>
-      <c r="J102" t="n">
+      <c r="K102" t="n">
         <v>37</v>
       </c>
-      <c r="K102" t="n">
+      <c r="L102" t="n">
         <v>0.01978999837013284</v>
       </c>
-      <c r="L102" t="n">
+      <c r="M102" t="n">
         <v>138.1836636194526</v>
       </c>
     </row>
@@ -4347,27 +4655,30 @@
         <v>11685</v>
       </c>
       <c r="E103" t="n">
+        <v>5320</v>
+      </c>
+      <c r="F103" t="n">
         <v>106968</v>
       </c>
-      <c r="F103" t="n">
+      <c r="G103" t="n">
         <v>483.4252786108728</v>
       </c>
-      <c r="G103" t="n">
+      <c r="H103" t="n">
         <v>0.04137144018920606</v>
       </c>
-      <c r="H103" t="n">
+      <c r="I103" t="n">
         <v>1.241143205676182</v>
       </c>
-      <c r="I103" t="n">
+      <c r="J103" t="n">
         <v>29.78743693622836</v>
       </c>
-      <c r="J103" t="n">
+      <c r="K103" t="n">
         <v>48</v>
       </c>
-      <c r="K103" t="n">
+      <c r="L103" t="n">
         <v>0.0141708709181092</v>
       </c>
-      <c r="L103" t="n">
+      <c r="M103" t="n">
         <v>165.586626678106</v>
       </c>
     </row>
@@ -4385,27 +4696,30 @@
         <v>3562.5</v>
       </c>
       <c r="E104" t="n">
+        <v>3752.5</v>
+      </c>
+      <c r="F104" t="n">
         <v>106968</v>
       </c>
-      <c r="F104" t="n">
+      <c r="G104" t="n">
         <v>266.9269563007828</v>
       </c>
-      <c r="G104" t="n">
+      <c r="H104" t="n">
         <v>0.07492686492653551</v>
       </c>
-      <c r="H104" t="n">
+      <c r="I104" t="n">
         <v>2.247805947796065</v>
       </c>
-      <c r="I104" t="n">
+      <c r="J104" t="n">
         <v>53.94734274710557</v>
       </c>
-      <c r="J104" t="n">
+      <c r="K104" t="n">
         <v>26</v>
       </c>
-      <c r="K104" t="n">
+      <c r="L104" t="n">
         <v>0.05190151191007675</v>
       </c>
-      <c r="L104" t="n">
+      <c r="M104" t="n">
         <v>184.8991361796484</v>
       </c>
     </row>

</xml_diff>